<commit_message>
error signal final update
</commit_message>
<xml_diff>
--- a/Figures/Final/raw/Raw Data.xlsx
+++ b/Figures/Final/raw/Raw Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertxi/Desktop/UChicago/Lab/Error Signal Simulation/Figures/Final/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572FEA12-ABF0-E048-A3FF-BCD5B31400EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C353C026-0B82-7F44-BDD8-5CC3D13FB242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28140" yWindow="500" windowWidth="23060" windowHeight="28300" xr2:uid="{D32071E5-1744-3348-B657-D312167DA67F}"/>
+    <workbookView xWindow="28140" yWindow="500" windowWidth="23060" windowHeight="28300" firstSheet="1" activeTab="6" xr2:uid="{D32071E5-1744-3348-B657-D312167DA67F}"/>
   </bookViews>
   <sheets>
     <sheet name="W a0 a1 Simulated 0.09" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Posi Scan After Field" sheetId="4" r:id="rId4"/>
     <sheet name="Posi Scan Mod Field" sheetId="5" r:id="rId5"/>
     <sheet name="W a0 a1 Anayltic 0.09" sheetId="6" r:id="rId6"/>
+    <sheet name="Long Posi Scan" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="141">
   <si>
     <t>a0</t>
   </si>
@@ -474,12 +475,225 @@
       <t>a1_analytic_mat = a1_analytic(cfg, E0_nr_values, detuning_L2_multipliers)</t>
     </r>
   </si>
+  <si>
+    <t>nr=160μs</t>
+  </si>
+  <si>
+    <t>nr=170μs</t>
+  </si>
+  <si>
+    <t>nr=180μs</t>
+  </si>
+  <si>
+    <t>nr=190μs</t>
+  </si>
+  <si>
+    <t>nr=200μs</t>
+  </si>
+  <si>
+    <t>nr=210μs</t>
+  </si>
+  <si>
+    <t>nr=220μs</t>
+  </si>
+  <si>
+    <t>nr=230μs</t>
+  </si>
+  <si>
+    <t>nr=240μs</t>
+  </si>
+  <si>
+    <t>nr=250μs</t>
+  </si>
+  <si>
+    <t>nr=260μs</t>
+  </si>
+  <si>
+    <t>nr=270μs</t>
+  </si>
+  <si>
+    <t>nr=280μs</t>
+  </si>
+  <si>
+    <t>nr=290μs</t>
+  </si>
+  <si>
+    <t>nr=300μs</t>
+  </si>
+  <si>
+    <t>nr=310μs</t>
+  </si>
+  <si>
+    <t>nr=320μs</t>
+  </si>
+  <si>
+    <t>nr=330μs</t>
+  </si>
+  <si>
+    <t>nr=340μs</t>
+  </si>
+  <si>
+    <t>nr=350μs</t>
+  </si>
+  <si>
+    <t>nr=360μs</t>
+  </si>
+  <si>
+    <t>nr=370μs</t>
+  </si>
+  <si>
+    <t>nr=380μs</t>
+  </si>
+  <si>
+    <t>nr=390μs</t>
+  </si>
+  <si>
+    <t>nr=400μs</t>
+  </si>
+  <si>
+    <t>nr=410μs</t>
+  </si>
+  <si>
+    <t>nr=420μs</t>
+  </si>
+  <si>
+    <t>nr=430μs</t>
+  </si>
+  <si>
+    <t>nr=440μs</t>
+  </si>
+  <si>
+    <t>nr=450μs</t>
+  </si>
+  <si>
+    <t>nr=460μs</t>
+  </si>
+  <si>
+    <t>nr=470μs</t>
+  </si>
+  <si>
+    <t>nr=480μs</t>
+  </si>
+  <si>
+    <t>nr=490μs</t>
+  </si>
+  <si>
+    <t>nr=500μs</t>
+  </si>
+  <si>
+    <t>nr=510μs</t>
+  </si>
+  <si>
+    <t>nr=520μs</t>
+  </si>
+  <si>
+    <t>nr=530μs</t>
+  </si>
+  <si>
+    <t>nr=540μs</t>
+  </si>
+  <si>
+    <t>nr=550μs</t>
+  </si>
+  <si>
+    <t>nr=560μs</t>
+  </si>
+  <si>
+    <t>nr=570μs</t>
+  </si>
+  <si>
+    <t>nr=580μs</t>
+  </si>
+  <si>
+    <t>nr=590μs</t>
+  </si>
+  <si>
+    <t>nr=600μs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nr_pos = 50:10:600; </t>
+  </si>
+  <si>
+    <t>L2_pos = 50:10:100;</t>
+  </si>
+  <si>
+    <t>cfg = SimConfig.default();</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cfg.t_nr = 120.1e-6; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF008013"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>% 70.1e-6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cfg.t_L2 = 102.6e-6; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF008013"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>% 52.6e-6</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg.detuning_L2 = 2*pi*1e6 * 3; </t>
+  </si>
+  <si>
+    <t>cfg.tspan = linspace(-51.1e-6,700e-6,10000);</t>
+  </si>
+  <si>
+    <t>cfg.detuning_range = linspace(-4000, 4000, 80) * 2*pi;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cfg.fieldMethod = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFA709F5"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>'default'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF008013"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>% 'before', 'after','modified','default'</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -531,6 +745,18 @@
       <b/>
       <sz val="13"/>
       <color rgb="FF0E00FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF008013"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFA709F5"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -1445,6 +1671,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>193579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A33A5F-8AED-F4C3-DCC1-86B2A926032A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6921500" y="5156200"/>
+          <a:ext cx="7772400" cy="1946179"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1764,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3E895A-9266-3844-B660-BEE330D90DEC}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
@@ -10086,4 +10361,4080 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5EA3C2-938E-E24F-95B4-DCC0C459EA6B}">
+  <dimension ref="A1:H197"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>29.306000000000001</v>
+      </c>
+      <c r="D5">
+        <v>13.391</v>
+      </c>
+      <c r="E5">
+        <v>5.6239999999999997</v>
+      </c>
+      <c r="F5">
+        <v>2.4213</v>
+      </c>
+      <c r="G5">
+        <v>1.0613999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.46557999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>45.828000000000003</v>
+      </c>
+      <c r="D6">
+        <v>29.390999999999998</v>
+      </c>
+      <c r="E6">
+        <v>13.532</v>
+      </c>
+      <c r="F6">
+        <v>5.6929999999999996</v>
+      </c>
+      <c r="G6">
+        <v>2.4396</v>
+      </c>
+      <c r="H6">
+        <v>1.0601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>53.08</v>
+      </c>
+      <c r="D7">
+        <v>45.366999999999997</v>
+      </c>
+      <c r="E7">
+        <v>29.213000000000001</v>
+      </c>
+      <c r="F7">
+        <v>13.526</v>
+      </c>
+      <c r="G7">
+        <v>5.6878000000000002</v>
+      </c>
+      <c r="H7">
+        <v>2.4213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>54.9</v>
+      </c>
+      <c r="D8">
+        <v>52.079000000000001</v>
+      </c>
+      <c r="E8">
+        <v>44.454999999999998</v>
+      </c>
+      <c r="F8">
+        <v>28.704999999999998</v>
+      </c>
+      <c r="G8">
+        <v>13.342000000000001</v>
+      </c>
+      <c r="H8">
+        <v>5.5960999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>54.453000000000003</v>
+      </c>
+      <c r="D9">
+        <v>53.329000000000001</v>
+      </c>
+      <c r="E9">
+        <v>50.476999999999997</v>
+      </c>
+      <c r="F9">
+        <v>43.000999999999998</v>
+      </c>
+      <c r="G9">
+        <v>27.811</v>
+      </c>
+      <c r="H9">
+        <v>12.952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>52.695999999999998</v>
+      </c>
+      <c r="D10">
+        <v>52.201999999999998</v>
+      </c>
+      <c r="E10">
+        <v>51.040999999999997</v>
+      </c>
+      <c r="F10">
+        <v>48.179000000000002</v>
+      </c>
+      <c r="G10">
+        <v>40.929000000000002</v>
+      </c>
+      <c r="H10">
+        <v>26.484000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>49.886000000000003</v>
+      </c>
+      <c r="D11">
+        <v>49.658000000000001</v>
+      </c>
+      <c r="E11">
+        <v>49.142000000000003</v>
+      </c>
+      <c r="F11">
+        <v>47.953000000000003</v>
+      </c>
+      <c r="G11">
+        <v>45.110999999999997</v>
+      </c>
+      <c r="H11">
+        <v>38.185000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>46.094999999999999</v>
+      </c>
+      <c r="D12">
+        <v>45.988</v>
+      </c>
+      <c r="E12">
+        <v>45.747999999999998</v>
+      </c>
+      <c r="F12">
+        <v>45.213000000000001</v>
+      </c>
+      <c r="G12">
+        <v>44.009</v>
+      </c>
+      <c r="H12">
+        <v>41.228999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>41.351999999999997</v>
+      </c>
+      <c r="D13">
+        <v>41.302</v>
+      </c>
+      <c r="E13">
+        <v>41.189</v>
+      </c>
+      <c r="F13">
+        <v>40.94</v>
+      </c>
+      <c r="G13">
+        <v>40.392000000000003</v>
+      </c>
+      <c r="H13">
+        <v>39.19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <v>35.695</v>
+      </c>
+      <c r="D14">
+        <v>35.670999999999999</v>
+      </c>
+      <c r="E14">
+        <v>35.618000000000002</v>
+      </c>
+      <c r="F14">
+        <v>35.5</v>
+      </c>
+      <c r="G14">
+        <v>35.244</v>
+      </c>
+      <c r="H14">
+        <v>34.692</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15">
+        <v>29.183</v>
+      </c>
+      <c r="D15">
+        <v>29.172000000000001</v>
+      </c>
+      <c r="E15">
+        <v>29.146999999999998</v>
+      </c>
+      <c r="F15">
+        <v>29.091999999999999</v>
+      </c>
+      <c r="G15">
+        <v>28.972000000000001</v>
+      </c>
+      <c r="H15">
+        <v>28.712</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>21.911000000000001</v>
+      </c>
+      <c r="D16">
+        <v>21.905999999999999</v>
+      </c>
+      <c r="E16">
+        <v>21.895</v>
+      </c>
+      <c r="F16">
+        <v>21.869</v>
+      </c>
+      <c r="G16">
+        <v>21.812999999999999</v>
+      </c>
+      <c r="H16">
+        <v>21.690999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17">
+        <v>14.007</v>
+      </c>
+      <c r="D17">
+        <v>14.005000000000001</v>
+      </c>
+      <c r="E17">
+        <v>13.999000000000001</v>
+      </c>
+      <c r="F17">
+        <v>13.988</v>
+      </c>
+      <c r="G17">
+        <v>13.961</v>
+      </c>
+      <c r="H17">
+        <v>13.904999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18">
+        <v>5.6276999999999999</v>
+      </c>
+      <c r="D18">
+        <v>5.6265999999999998</v>
+      </c>
+      <c r="E18">
+        <v>5.6242000000000001</v>
+      </c>
+      <c r="F18">
+        <v>5.6186999999999996</v>
+      </c>
+      <c r="G18">
+        <v>5.6067</v>
+      </c>
+      <c r="H18">
+        <v>5.5803000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19">
+        <v>-3.0442</v>
+      </c>
+      <c r="D19">
+        <v>-3.0447000000000002</v>
+      </c>
+      <c r="E19">
+        <v>-3.0457999999999998</v>
+      </c>
+      <c r="F19">
+        <v>-3.0482999999999998</v>
+      </c>
+      <c r="G19">
+        <v>-3.0537999999999998</v>
+      </c>
+      <c r="H19">
+        <v>-3.0659000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20">
+        <v>-11.808</v>
+      </c>
+      <c r="D20">
+        <v>-11.808</v>
+      </c>
+      <c r="E20">
+        <v>-11.808999999999999</v>
+      </c>
+      <c r="F20">
+        <v>-11.81</v>
+      </c>
+      <c r="G20">
+        <v>-11.811999999999999</v>
+      </c>
+      <c r="H20">
+        <v>-11.818</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21">
+        <v>-20.452999999999999</v>
+      </c>
+      <c r="D21">
+        <v>-20.452999999999999</v>
+      </c>
+      <c r="E21">
+        <v>-20.452999999999999</v>
+      </c>
+      <c r="F21">
+        <v>-20.454000000000001</v>
+      </c>
+      <c r="G21">
+        <v>-20.454999999999998</v>
+      </c>
+      <c r="H21">
+        <v>-20.457999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22">
+        <v>-28.768999999999998</v>
+      </c>
+      <c r="D22">
+        <v>-28.768999999999998</v>
+      </c>
+      <c r="E22">
+        <v>-28.768999999999998</v>
+      </c>
+      <c r="F22">
+        <v>-28.768999999999998</v>
+      </c>
+      <c r="G22">
+        <v>-28.77</v>
+      </c>
+      <c r="H22">
+        <v>-28.771000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>-36.552999999999997</v>
+      </c>
+      <c r="D23">
+        <v>-36.552999999999997</v>
+      </c>
+      <c r="E23">
+        <v>-36.552999999999997</v>
+      </c>
+      <c r="F23">
+        <v>-36.552999999999997</v>
+      </c>
+      <c r="G23">
+        <v>-36.554000000000002</v>
+      </c>
+      <c r="H23">
+        <v>-36.554000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24">
+        <v>-43.621000000000002</v>
+      </c>
+      <c r="D24">
+        <v>-43.621000000000002</v>
+      </c>
+      <c r="E24">
+        <v>-43.621000000000002</v>
+      </c>
+      <c r="F24">
+        <v>-43.621000000000002</v>
+      </c>
+      <c r="G24">
+        <v>-43.621000000000002</v>
+      </c>
+      <c r="H24">
+        <v>-43.621000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25">
+        <v>-49.811</v>
+      </c>
+      <c r="D25">
+        <v>-49.811</v>
+      </c>
+      <c r="E25">
+        <v>-49.811</v>
+      </c>
+      <c r="F25">
+        <v>-49.811</v>
+      </c>
+      <c r="G25">
+        <v>-49.811</v>
+      </c>
+      <c r="H25">
+        <v>-49.811999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26">
+        <v>-54.997</v>
+      </c>
+      <c r="D26">
+        <v>-54.997</v>
+      </c>
+      <c r="E26">
+        <v>-54.997</v>
+      </c>
+      <c r="F26">
+        <v>-54.997</v>
+      </c>
+      <c r="G26">
+        <v>-54.997</v>
+      </c>
+      <c r="H26">
+        <v>-54.997999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27">
+        <v>-59.088000000000001</v>
+      </c>
+      <c r="D27">
+        <v>-59.088000000000001</v>
+      </c>
+      <c r="E27">
+        <v>-59.088000000000001</v>
+      </c>
+      <c r="F27">
+        <v>-59.088000000000001</v>
+      </c>
+      <c r="G27">
+        <v>-59.088000000000001</v>
+      </c>
+      <c r="H27">
+        <v>-59.088000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28">
+        <v>-62.030999999999999</v>
+      </c>
+      <c r="D28">
+        <v>-62.030999999999999</v>
+      </c>
+      <c r="E28">
+        <v>-62.030999999999999</v>
+      </c>
+      <c r="F28">
+        <v>-62.030999999999999</v>
+      </c>
+      <c r="G28">
+        <v>-62.030999999999999</v>
+      </c>
+      <c r="H28">
+        <v>-62.031999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29">
+        <v>-63.819000000000003</v>
+      </c>
+      <c r="D29">
+        <v>-63.819000000000003</v>
+      </c>
+      <c r="E29">
+        <v>-63.819000000000003</v>
+      </c>
+      <c r="F29">
+        <v>-63.819000000000003</v>
+      </c>
+      <c r="G29">
+        <v>-63.819000000000003</v>
+      </c>
+      <c r="H29">
+        <v>-63.819000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30">
+        <v>-64.481999999999999</v>
+      </c>
+      <c r="D30">
+        <v>-64.481999999999999</v>
+      </c>
+      <c r="E30">
+        <v>-64.481999999999999</v>
+      </c>
+      <c r="F30">
+        <v>-64.481999999999999</v>
+      </c>
+      <c r="G30">
+        <v>-64.481999999999999</v>
+      </c>
+      <c r="H30">
+        <v>-64.481999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31">
+        <v>-64.09</v>
+      </c>
+      <c r="D31">
+        <v>-64.09</v>
+      </c>
+      <c r="E31">
+        <v>-64.09</v>
+      </c>
+      <c r="F31">
+        <v>-64.09</v>
+      </c>
+      <c r="G31">
+        <v>-64.09</v>
+      </c>
+      <c r="H31">
+        <v>-64.09</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32">
+        <v>-62.744999999999997</v>
+      </c>
+      <c r="D32">
+        <v>-62.744999999999997</v>
+      </c>
+      <c r="E32">
+        <v>-62.744999999999997</v>
+      </c>
+      <c r="F32">
+        <v>-62.744999999999997</v>
+      </c>
+      <c r="G32">
+        <v>-62.744999999999997</v>
+      </c>
+      <c r="H32">
+        <v>-62.744999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33">
+        <v>-60.576999999999998</v>
+      </c>
+      <c r="D33">
+        <v>-60.576999999999998</v>
+      </c>
+      <c r="E33">
+        <v>-60.576999999999998</v>
+      </c>
+      <c r="F33">
+        <v>-60.576999999999998</v>
+      </c>
+      <c r="G33">
+        <v>-60.576999999999998</v>
+      </c>
+      <c r="H33">
+        <v>-60.576999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34">
+        <v>-57.738999999999997</v>
+      </c>
+      <c r="D34">
+        <v>-57.738999999999997</v>
+      </c>
+      <c r="E34">
+        <v>-57.738999999999997</v>
+      </c>
+      <c r="F34">
+        <v>-57.738999999999997</v>
+      </c>
+      <c r="G34">
+        <v>-57.738999999999997</v>
+      </c>
+      <c r="H34">
+        <v>-57.738999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35">
+        <v>-54.393000000000001</v>
+      </c>
+      <c r="D35">
+        <v>-54.393000000000001</v>
+      </c>
+      <c r="E35">
+        <v>-54.393000000000001</v>
+      </c>
+      <c r="F35">
+        <v>-54.393000000000001</v>
+      </c>
+      <c r="G35">
+        <v>-54.393000000000001</v>
+      </c>
+      <c r="H35">
+        <v>-54.393000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36">
+        <v>-50.707000000000001</v>
+      </c>
+      <c r="D36">
+        <v>-50.707000000000001</v>
+      </c>
+      <c r="E36">
+        <v>-50.707000000000001</v>
+      </c>
+      <c r="F36">
+        <v>-50.707000000000001</v>
+      </c>
+      <c r="G36">
+        <v>-50.707000000000001</v>
+      </c>
+      <c r="H36">
+        <v>-50.707000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37">
+        <v>-46.844999999999999</v>
+      </c>
+      <c r="D37">
+        <v>-46.844999999999999</v>
+      </c>
+      <c r="E37">
+        <v>-46.844999999999999</v>
+      </c>
+      <c r="F37">
+        <v>-46.844999999999999</v>
+      </c>
+      <c r="G37">
+        <v>-46.844999999999999</v>
+      </c>
+      <c r="H37">
+        <v>-46.844999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38">
+        <v>-42.96</v>
+      </c>
+      <c r="D38">
+        <v>-42.96</v>
+      </c>
+      <c r="E38">
+        <v>-42.96</v>
+      </c>
+      <c r="F38">
+        <v>-42.96</v>
+      </c>
+      <c r="G38">
+        <v>-42.96</v>
+      </c>
+      <c r="H38">
+        <v>-42.96</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39">
+        <v>-39.185000000000002</v>
+      </c>
+      <c r="D39">
+        <v>-39.185000000000002</v>
+      </c>
+      <c r="E39">
+        <v>-39.185000000000002</v>
+      </c>
+      <c r="F39">
+        <v>-39.185000000000002</v>
+      </c>
+      <c r="G39">
+        <v>-39.185000000000002</v>
+      </c>
+      <c r="H39">
+        <v>-39.185000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40">
+        <v>-35.631999999999998</v>
+      </c>
+      <c r="D40">
+        <v>-35.631999999999998</v>
+      </c>
+      <c r="E40">
+        <v>-35.631999999999998</v>
+      </c>
+      <c r="F40">
+        <v>-35.631999999999998</v>
+      </c>
+      <c r="G40">
+        <v>-35.631999999999998</v>
+      </c>
+      <c r="H40">
+        <v>-35.631999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41">
+        <v>-32.384</v>
+      </c>
+      <c r="D41">
+        <v>-32.384</v>
+      </c>
+      <c r="E41">
+        <v>-32.384</v>
+      </c>
+      <c r="F41">
+        <v>-32.384</v>
+      </c>
+      <c r="G41">
+        <v>-32.384</v>
+      </c>
+      <c r="H41">
+        <v>-32.384</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42">
+        <v>-29.494</v>
+      </c>
+      <c r="D42">
+        <v>-29.494</v>
+      </c>
+      <c r="E42">
+        <v>-29.494</v>
+      </c>
+      <c r="F42">
+        <v>-29.494</v>
+      </c>
+      <c r="G42">
+        <v>-29.494</v>
+      </c>
+      <c r="H42">
+        <v>-29.494</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43">
+        <v>-26.984999999999999</v>
+      </c>
+      <c r="D43">
+        <v>-26.984999999999999</v>
+      </c>
+      <c r="E43">
+        <v>-26.984999999999999</v>
+      </c>
+      <c r="F43">
+        <v>-26.984999999999999</v>
+      </c>
+      <c r="G43">
+        <v>-26.984999999999999</v>
+      </c>
+      <c r="H43">
+        <v>-26.984999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44">
+        <v>-24.85</v>
+      </c>
+      <c r="D44">
+        <v>-24.85</v>
+      </c>
+      <c r="E44">
+        <v>-24.85</v>
+      </c>
+      <c r="F44">
+        <v>-24.85</v>
+      </c>
+      <c r="G44">
+        <v>-24.85</v>
+      </c>
+      <c r="H44">
+        <v>-24.85</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45">
+        <v>-23.056000000000001</v>
+      </c>
+      <c r="D45">
+        <v>-23.056000000000001</v>
+      </c>
+      <c r="E45">
+        <v>-23.056000000000001</v>
+      </c>
+      <c r="F45">
+        <v>-23.056000000000001</v>
+      </c>
+      <c r="G45">
+        <v>-23.056000000000001</v>
+      </c>
+      <c r="H45">
+        <v>-23.056000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46">
+        <v>-21.547999999999998</v>
+      </c>
+      <c r="D46">
+        <v>-21.547999999999998</v>
+      </c>
+      <c r="E46">
+        <v>-21.547999999999998</v>
+      </c>
+      <c r="F46">
+        <v>-21.547999999999998</v>
+      </c>
+      <c r="G46">
+        <v>-21.547999999999998</v>
+      </c>
+      <c r="H46">
+        <v>-21.547999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47">
+        <v>-20.251000000000001</v>
+      </c>
+      <c r="D47">
+        <v>-20.251000000000001</v>
+      </c>
+      <c r="E47">
+        <v>-20.251000000000001</v>
+      </c>
+      <c r="F47">
+        <v>-20.251000000000001</v>
+      </c>
+      <c r="G47">
+        <v>-20.251000000000001</v>
+      </c>
+      <c r="H47">
+        <v>-20.251000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48">
+        <v>-19.081</v>
+      </c>
+      <c r="D48">
+        <v>-19.081</v>
+      </c>
+      <c r="E48">
+        <v>-19.081</v>
+      </c>
+      <c r="F48">
+        <v>-19.081</v>
+      </c>
+      <c r="G48">
+        <v>-19.081</v>
+      </c>
+      <c r="H48">
+        <v>-19.081</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49">
+        <v>-17.949000000000002</v>
+      </c>
+      <c r="D49">
+        <v>-17.949000000000002</v>
+      </c>
+      <c r="E49">
+        <v>-17.949000000000002</v>
+      </c>
+      <c r="F49">
+        <v>-17.949000000000002</v>
+      </c>
+      <c r="G49">
+        <v>-17.949000000000002</v>
+      </c>
+      <c r="H49">
+        <v>-17.949000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50">
+        <v>-16.765000000000001</v>
+      </c>
+      <c r="D50">
+        <v>-16.765000000000001</v>
+      </c>
+      <c r="E50">
+        <v>-16.765000000000001</v>
+      </c>
+      <c r="F50">
+        <v>-16.765000000000001</v>
+      </c>
+      <c r="G50">
+        <v>-16.765000000000001</v>
+      </c>
+      <c r="H50">
+        <v>-16.765000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51">
+        <v>-15.446999999999999</v>
+      </c>
+      <c r="D51">
+        <v>-15.446999999999999</v>
+      </c>
+      <c r="E51">
+        <v>-15.446999999999999</v>
+      </c>
+      <c r="F51">
+        <v>-15.446999999999999</v>
+      </c>
+      <c r="G51">
+        <v>-15.446999999999999</v>
+      </c>
+      <c r="H51">
+        <v>-15.446999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52">
+        <v>-13.926</v>
+      </c>
+      <c r="D52">
+        <v>-13.926</v>
+      </c>
+      <c r="E52">
+        <v>-13.926</v>
+      </c>
+      <c r="F52">
+        <v>-13.926</v>
+      </c>
+      <c r="G52">
+        <v>-13.926</v>
+      </c>
+      <c r="H52">
+        <v>-13.926</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53">
+        <v>-12.15</v>
+      </c>
+      <c r="D53">
+        <v>-12.15</v>
+      </c>
+      <c r="E53">
+        <v>-12.15</v>
+      </c>
+      <c r="F53">
+        <v>-12.15</v>
+      </c>
+      <c r="G53">
+        <v>-12.15</v>
+      </c>
+      <c r="H53">
+        <v>-12.15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54">
+        <v>-10.085000000000001</v>
+      </c>
+      <c r="D54">
+        <v>-10.085000000000001</v>
+      </c>
+      <c r="E54">
+        <v>-10.085000000000001</v>
+      </c>
+      <c r="F54">
+        <v>-10.085000000000001</v>
+      </c>
+      <c r="G54">
+        <v>-10.085000000000001</v>
+      </c>
+      <c r="H54">
+        <v>-10.085000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55">
+        <v>-7.7217000000000002</v>
+      </c>
+      <c r="D55">
+        <v>-7.7217000000000002</v>
+      </c>
+      <c r="E55">
+        <v>-7.7217000000000002</v>
+      </c>
+      <c r="F55">
+        <v>-7.7217000000000002</v>
+      </c>
+      <c r="G55">
+        <v>-7.7217000000000002</v>
+      </c>
+      <c r="H55">
+        <v>-7.7217000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56">
+        <v>-5.0709999999999997</v>
+      </c>
+      <c r="D56">
+        <v>-5.0709999999999997</v>
+      </c>
+      <c r="E56">
+        <v>-5.0709999999999997</v>
+      </c>
+      <c r="F56">
+        <v>-5.0709999999999997</v>
+      </c>
+      <c r="G56">
+        <v>-5.0709999999999997</v>
+      </c>
+      <c r="H56">
+        <v>-5.0709999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57">
+        <v>-2.1657999999999999</v>
+      </c>
+      <c r="D57">
+        <v>-2.1657999999999999</v>
+      </c>
+      <c r="E57">
+        <v>-2.1657999999999999</v>
+      </c>
+      <c r="F57">
+        <v>-2.1657999999999999</v>
+      </c>
+      <c r="G57">
+        <v>-2.1657999999999999</v>
+      </c>
+      <c r="H57">
+        <v>-2.1657999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58">
+        <v>0.94181000000000004</v>
+      </c>
+      <c r="D58">
+        <v>0.94181000000000004</v>
+      </c>
+      <c r="E58">
+        <v>0.94181000000000004</v>
+      </c>
+      <c r="F58">
+        <v>0.94181000000000004</v>
+      </c>
+      <c r="G58">
+        <v>0.94181000000000004</v>
+      </c>
+      <c r="H58">
+        <v>0.94181000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="D59">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="E59">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="F59">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="G59">
+        <v>4.1840000000000002</v>
+      </c>
+      <c r="H59">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>131</v>
+      </c>
+      <c r="C60">
+        <v>7.4805999999999999</v>
+      </c>
+      <c r="D60">
+        <v>7.4805999999999999</v>
+      </c>
+      <c r="E60">
+        <v>7.4805999999999999</v>
+      </c>
+      <c r="F60">
+        <v>7.4805999999999999</v>
+      </c>
+      <c r="G60">
+        <v>7.4805999999999999</v>
+      </c>
+      <c r="H60">
+        <v>7.4805999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" t="s">
+        <v>36</v>
+      </c>
+      <c r="G63" t="s">
+        <v>37</v>
+      </c>
+      <c r="H63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66">
+        <v>-0.29176000000000002</v>
+      </c>
+      <c r="D66">
+        <v>-0.42297000000000001</v>
+      </c>
+      <c r="E66">
+        <v>-0.49519999999999997</v>
+      </c>
+      <c r="F66">
+        <v>-0.52903999999999995</v>
+      </c>
+      <c r="G66">
+        <v>-0.54468000000000005</v>
+      </c>
+      <c r="H66">
+        <v>-0.55186000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67">
+        <v>-0.18904000000000001</v>
+      </c>
+      <c r="D67">
+        <v>-0.35525000000000001</v>
+      </c>
+      <c r="E67">
+        <v>-0.50017999999999996</v>
+      </c>
+      <c r="F67">
+        <v>-0.57474999999999998</v>
+      </c>
+      <c r="G67">
+        <v>-0.60768</v>
+      </c>
+      <c r="H67">
+        <v>-0.62222</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68">
+        <v>-0.10789</v>
+      </c>
+      <c r="D68">
+        <v>-0.22331000000000001</v>
+      </c>
+      <c r="E68">
+        <v>-0.40888000000000002</v>
+      </c>
+      <c r="F68">
+        <v>-0.56286999999999998</v>
+      </c>
+      <c r="G68">
+        <v>-0.63729000000000002</v>
+      </c>
+      <c r="H68">
+        <v>-0.66822000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69">
+        <v>-6.608E-2</v>
+      </c>
+      <c r="D69">
+        <v>-0.12361999999999999</v>
+      </c>
+      <c r="E69">
+        <v>-0.25158000000000003</v>
+      </c>
+      <c r="F69">
+        <v>-0.45112999999999998</v>
+      </c>
+      <c r="G69">
+        <v>-0.60943000000000003</v>
+      </c>
+      <c r="H69">
+        <v>-0.68128999999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70">
+        <v>-4.6841000000000001E-2</v>
+      </c>
+      <c r="D70">
+        <v>-7.2942000000000007E-2</v>
+      </c>
+      <c r="E70">
+        <v>-0.13611999999999999</v>
+      </c>
+      <c r="F70">
+        <v>-0.27312999999999998</v>
+      </c>
+      <c r="G70">
+        <v>-0.48107</v>
+      </c>
+      <c r="H70">
+        <v>-0.63895000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71">
+        <v>-3.7941999999999997E-2</v>
+      </c>
+      <c r="D71">
+        <v>-4.9506000000000001E-2</v>
+      </c>
+      <c r="E71">
+        <v>-7.7949000000000004E-2</v>
+      </c>
+      <c r="F71">
+        <v>-0.14507</v>
+      </c>
+      <c r="G71">
+        <v>-0.28752</v>
+      </c>
+      <c r="H71">
+        <v>-0.49823000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72">
+        <v>-3.3353000000000001E-2</v>
+      </c>
+      <c r="D72">
+        <v>-3.8427999999999997E-2</v>
+      </c>
+      <c r="E72">
+        <v>-5.0966999999999998E-2</v>
+      </c>
+      <c r="F72">
+        <v>-8.1002000000000005E-2</v>
+      </c>
+      <c r="G72">
+        <v>-0.15032999999999999</v>
+      </c>
+      <c r="H72">
+        <v>-0.29459000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73">
+        <v>-3.0339999999999999E-2</v>
+      </c>
+      <c r="D73">
+        <v>-3.2552999999999999E-2</v>
+      </c>
+      <c r="E73">
+        <v>-3.8041999999999999E-2</v>
+      </c>
+      <c r="F73">
+        <v>-5.1229999999999998E-2</v>
+      </c>
+      <c r="G73">
+        <v>-8.2086999999999993E-2</v>
+      </c>
+      <c r="H73">
+        <v>-0.15190000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74">
+        <v>-2.7730000000000001E-2</v>
+      </c>
+      <c r="D74">
+        <v>-2.8691999999999999E-2</v>
+      </c>
+      <c r="E74">
+        <v>-3.1084000000000001E-2</v>
+      </c>
+      <c r="F74">
+        <v>-3.6843000000000001E-2</v>
+      </c>
+      <c r="G74">
+        <v>-5.0345000000000001E-2</v>
+      </c>
+      <c r="H74">
+        <v>-8.1262000000000001E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75">
+        <v>-2.5068E-2</v>
+      </c>
+      <c r="D75">
+        <v>-2.5485000000000001E-2</v>
+      </c>
+      <c r="E75">
+        <v>-2.6525E-2</v>
+      </c>
+      <c r="F75">
+        <v>-2.9034000000000001E-2</v>
+      </c>
+      <c r="G75">
+        <v>-3.4918999999999999E-2</v>
+      </c>
+      <c r="H75">
+        <v>-4.8401E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76">
+        <v>-2.2225000000000002E-2</v>
+      </c>
+      <c r="D76">
+        <v>-2.2405000000000001E-2</v>
+      </c>
+      <c r="E76">
+        <v>-2.2856999999999999E-2</v>
+      </c>
+      <c r="F76">
+        <v>-2.3948000000000001E-2</v>
+      </c>
+      <c r="G76">
+        <v>-2.6509999999999999E-2</v>
+      </c>
+      <c r="H76">
+        <v>-3.2375000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77">
+        <v>-1.9213999999999998E-2</v>
+      </c>
+      <c r="D77">
+        <v>-1.9292E-2</v>
+      </c>
+      <c r="E77">
+        <v>-1.9487999999999998E-2</v>
+      </c>
+      <c r="F77">
+        <v>-1.9963000000000002E-2</v>
+      </c>
+      <c r="G77">
+        <v>-2.1076999999999999E-2</v>
+      </c>
+      <c r="H77">
+        <v>-2.3629000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78">
+        <v>-1.6111E-2</v>
+      </c>
+      <c r="D78">
+        <v>-1.6145E-2</v>
+      </c>
+      <c r="E78">
+        <v>-1.6230000000000001E-2</v>
+      </c>
+      <c r="F78">
+        <v>-1.6437E-2</v>
+      </c>
+      <c r="G78">
+        <v>-1.6922E-2</v>
+      </c>
+      <c r="H78">
+        <v>-1.8031999999999999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79">
+        <v>-1.3013E-2</v>
+      </c>
+      <c r="D79">
+        <v>-1.3028E-2</v>
+      </c>
+      <c r="E79">
+        <v>-1.3065E-2</v>
+      </c>
+      <c r="F79">
+        <v>-1.3155E-2</v>
+      </c>
+      <c r="G79">
+        <v>-1.3367E-2</v>
+      </c>
+      <c r="H79">
+        <v>-1.3851E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80">
+        <v>-1.0019999999999999E-2</v>
+      </c>
+      <c r="D80">
+        <v>-1.0026999999999999E-2</v>
+      </c>
+      <c r="E80">
+        <v>-1.0043E-2</v>
+      </c>
+      <c r="F80">
+        <v>-1.0082000000000001E-2</v>
+      </c>
+      <c r="G80">
+        <v>-1.0175E-2</v>
+      </c>
+      <c r="H80">
+        <v>-1.0385999999999999E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81">
+        <v>-7.2227000000000003E-3</v>
+      </c>
+      <c r="D81">
+        <v>-7.2255000000000002E-3</v>
+      </c>
+      <c r="E81">
+        <v>-7.2325999999999996E-3</v>
+      </c>
+      <c r="F81">
+        <v>-7.2497999999999998E-3</v>
+      </c>
+      <c r="G81">
+        <v>-7.2902000000000002E-3</v>
+      </c>
+      <c r="H81">
+        <v>-7.3823999999999999E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82">
+        <v>-4.6962000000000002E-3</v>
+      </c>
+      <c r="D82">
+        <v>-4.6975000000000003E-3</v>
+      </c>
+      <c r="E82">
+        <v>-4.7006000000000001E-3</v>
+      </c>
+      <c r="F82">
+        <v>-4.7080999999999998E-3</v>
+      </c>
+      <c r="G82">
+        <v>-4.7257000000000002E-3</v>
+      </c>
+      <c r="H82">
+        <v>-4.7660999999999997E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83">
+        <v>-2.4987E-3</v>
+      </c>
+      <c r="D83">
+        <v>-2.4992E-3</v>
+      </c>
+      <c r="E83">
+        <v>-2.5006E-3</v>
+      </c>
+      <c r="F83">
+        <v>-2.5038999999999999E-3</v>
+      </c>
+      <c r="G83">
+        <v>-2.5116000000000001E-3</v>
+      </c>
+      <c r="H83">
+        <v>-2.5293E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84">
+        <v>-6.6774E-4</v>
+      </c>
+      <c r="D84">
+        <v>-6.6797000000000004E-4</v>
+      </c>
+      <c r="E84">
+        <v>-6.6856999999999995E-4</v>
+      </c>
+      <c r="F84">
+        <v>-6.7000999999999996E-4</v>
+      </c>
+      <c r="G84">
+        <v>-6.734E-4</v>
+      </c>
+      <c r="H84">
+        <v>-6.8112999999999995E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85">
+        <v>7.7976E-4</v>
+      </c>
+      <c r="D85">
+        <v>7.7965E-4</v>
+      </c>
+      <c r="E85">
+        <v>7.7939000000000003E-4</v>
+      </c>
+      <c r="F85">
+        <v>7.7875999999999998E-4</v>
+      </c>
+      <c r="G85">
+        <v>7.7727999999999998E-4</v>
+      </c>
+      <c r="H85">
+        <v>7.7388999999999995E-4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86">
+        <v>1.8469999999999999E-3</v>
+      </c>
+      <c r="D86">
+        <v>1.8469000000000001E-3</v>
+      </c>
+      <c r="E86">
+        <v>1.8468E-3</v>
+      </c>
+      <c r="F86">
+        <v>1.8465000000000001E-3</v>
+      </c>
+      <c r="G86">
+        <v>1.8458999999999999E-3</v>
+      </c>
+      <c r="H86">
+        <v>1.8443999999999999E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87">
+        <v>2.5555999999999999E-3</v>
+      </c>
+      <c r="D87">
+        <v>2.5555999999999999E-3</v>
+      </c>
+      <c r="E87">
+        <v>2.5555E-3</v>
+      </c>
+      <c r="F87">
+        <v>2.5554000000000002E-3</v>
+      </c>
+      <c r="G87">
+        <v>2.5550999999999998E-3</v>
+      </c>
+      <c r="H87">
+        <v>2.5544999999999999E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>98</v>
+      </c>
+      <c r="C88">
+        <v>2.9432E-3</v>
+      </c>
+      <c r="D88">
+        <v>2.9432E-3</v>
+      </c>
+      <c r="E88">
+        <v>2.9431000000000001E-3</v>
+      </c>
+      <c r="F88">
+        <v>2.9431000000000001E-3</v>
+      </c>
+      <c r="G88">
+        <v>2.9429999999999999E-3</v>
+      </c>
+      <c r="H88">
+        <v>2.9426999999999999E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89">
+        <v>3.0601000000000001E-3</v>
+      </c>
+      <c r="D89">
+        <v>3.0601000000000001E-3</v>
+      </c>
+      <c r="E89">
+        <v>3.0601000000000001E-3</v>
+      </c>
+      <c r="F89">
+        <v>3.0601000000000001E-3</v>
+      </c>
+      <c r="G89">
+        <v>3.0599999999999998E-3</v>
+      </c>
+      <c r="H89">
+        <v>3.0598999999999999E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90">
+        <v>2.9659999999999999E-3</v>
+      </c>
+      <c r="D90">
+        <v>2.9659999999999999E-3</v>
+      </c>
+      <c r="E90">
+        <v>2.9659E-3</v>
+      </c>
+      <c r="F90">
+        <v>2.9659E-3</v>
+      </c>
+      <c r="G90">
+        <v>2.9659E-3</v>
+      </c>
+      <c r="H90">
+        <v>2.9659E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91">
+        <v>2.7253999999999998E-3</v>
+      </c>
+      <c r="D91">
+        <v>2.7253999999999998E-3</v>
+      </c>
+      <c r="E91">
+        <v>2.7253999999999998E-3</v>
+      </c>
+      <c r="F91">
+        <v>2.7253999999999998E-3</v>
+      </c>
+      <c r="G91">
+        <v>2.7253999999999998E-3</v>
+      </c>
+      <c r="H91">
+        <v>2.7253999999999998E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92">
+        <v>2.4044000000000001E-3</v>
+      </c>
+      <c r="D92">
+        <v>2.4044000000000001E-3</v>
+      </c>
+      <c r="E92">
+        <v>2.4044000000000001E-3</v>
+      </c>
+      <c r="F92">
+        <v>2.4044000000000001E-3</v>
+      </c>
+      <c r="G92">
+        <v>2.4044000000000001E-3</v>
+      </c>
+      <c r="H92">
+        <v>2.4044000000000001E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93">
+        <v>2.0663999999999999E-3</v>
+      </c>
+      <c r="D93">
+        <v>2.0663999999999999E-3</v>
+      </c>
+      <c r="E93">
+        <v>2.0663999999999999E-3</v>
+      </c>
+      <c r="F93">
+        <v>2.0663999999999999E-3</v>
+      </c>
+      <c r="G93">
+        <v>2.0663999999999999E-3</v>
+      </c>
+      <c r="H93">
+        <v>2.0663999999999999E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>104</v>
+      </c>
+      <c r="C94">
+        <v>1.7688000000000001E-3</v>
+      </c>
+      <c r="D94">
+        <v>1.7688000000000001E-3</v>
+      </c>
+      <c r="E94">
+        <v>1.7688000000000001E-3</v>
+      </c>
+      <c r="F94">
+        <v>1.7688000000000001E-3</v>
+      </c>
+      <c r="G94">
+        <v>1.7688000000000001E-3</v>
+      </c>
+      <c r="H94">
+        <v>1.7688000000000001E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>105</v>
+      </c>
+      <c r="C95">
+        <v>1.56E-3</v>
+      </c>
+      <c r="D95">
+        <v>1.56E-3</v>
+      </c>
+      <c r="E95">
+        <v>1.56E-3</v>
+      </c>
+      <c r="F95">
+        <v>1.56E-3</v>
+      </c>
+      <c r="G95">
+        <v>1.56E-3</v>
+      </c>
+      <c r="H95">
+        <v>1.56E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96">
+        <v>1.4774E-3</v>
+      </c>
+      <c r="D96">
+        <v>1.4774E-3</v>
+      </c>
+      <c r="E96">
+        <v>1.4774E-3</v>
+      </c>
+      <c r="F96">
+        <v>1.4774E-3</v>
+      </c>
+      <c r="G96">
+        <v>1.4774E-3</v>
+      </c>
+      <c r="H96">
+        <v>1.4774E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>107</v>
+      </c>
+      <c r="C97">
+        <v>1.5456999999999999E-3</v>
+      </c>
+      <c r="D97">
+        <v>1.5456999999999999E-3</v>
+      </c>
+      <c r="E97">
+        <v>1.5456999999999999E-3</v>
+      </c>
+      <c r="F97">
+        <v>1.5456999999999999E-3</v>
+      </c>
+      <c r="G97">
+        <v>1.5456999999999999E-3</v>
+      </c>
+      <c r="H97">
+        <v>1.5456999999999999E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98">
+        <v>1.7763E-3</v>
+      </c>
+      <c r="D98">
+        <v>1.7763E-3</v>
+      </c>
+      <c r="E98">
+        <v>1.7763E-3</v>
+      </c>
+      <c r="F98">
+        <v>1.7763E-3</v>
+      </c>
+      <c r="G98">
+        <v>1.7763E-3</v>
+      </c>
+      <c r="H98">
+        <v>1.7763E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99">
+        <v>2.1673999999999999E-3</v>
+      </c>
+      <c r="D99">
+        <v>2.1673999999999999E-3</v>
+      </c>
+      <c r="E99">
+        <v>2.1673999999999999E-3</v>
+      </c>
+      <c r="F99">
+        <v>2.1673999999999999E-3</v>
+      </c>
+      <c r="G99">
+        <v>2.1673999999999999E-3</v>
+      </c>
+      <c r="H99">
+        <v>2.1673999999999999E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100">
+        <v>2.7049999999999999E-3</v>
+      </c>
+      <c r="D100">
+        <v>2.7049999999999999E-3</v>
+      </c>
+      <c r="E100">
+        <v>2.7049999999999999E-3</v>
+      </c>
+      <c r="F100">
+        <v>2.7049999999999999E-3</v>
+      </c>
+      <c r="G100">
+        <v>2.7049999999999999E-3</v>
+      </c>
+      <c r="H100">
+        <v>2.7049999999999999E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>111</v>
+      </c>
+      <c r="C101">
+        <v>3.3643000000000002E-3</v>
+      </c>
+      <c r="D101">
+        <v>3.3643000000000002E-3</v>
+      </c>
+      <c r="E101">
+        <v>3.3643000000000002E-3</v>
+      </c>
+      <c r="F101">
+        <v>3.3643000000000002E-3</v>
+      </c>
+      <c r="G101">
+        <v>3.3643000000000002E-3</v>
+      </c>
+      <c r="H101">
+        <v>3.3643000000000002E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>112</v>
+      </c>
+      <c r="C102">
+        <v>4.1117999999999997E-3</v>
+      </c>
+      <c r="D102">
+        <v>4.1117999999999997E-3</v>
+      </c>
+      <c r="E102">
+        <v>4.1117999999999997E-3</v>
+      </c>
+      <c r="F102">
+        <v>4.1117999999999997E-3</v>
+      </c>
+      <c r="G102">
+        <v>4.1117999999999997E-3</v>
+      </c>
+      <c r="H102">
+        <v>4.1117999999999997E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>113</v>
+      </c>
+      <c r="C103">
+        <v>4.9081000000000003E-3</v>
+      </c>
+      <c r="D103">
+        <v>4.9081000000000003E-3</v>
+      </c>
+      <c r="E103">
+        <v>4.9081000000000003E-3</v>
+      </c>
+      <c r="F103">
+        <v>4.9081000000000003E-3</v>
+      </c>
+      <c r="G103">
+        <v>4.9081000000000003E-3</v>
+      </c>
+      <c r="H103">
+        <v>4.9081000000000003E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>114</v>
+      </c>
+      <c r="C104">
+        <v>5.7104E-3</v>
+      </c>
+      <c r="D104">
+        <v>5.7104E-3</v>
+      </c>
+      <c r="E104">
+        <v>5.7104E-3</v>
+      </c>
+      <c r="F104">
+        <v>5.7104E-3</v>
+      </c>
+      <c r="G104">
+        <v>5.7104E-3</v>
+      </c>
+      <c r="H104">
+        <v>5.7104E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105">
+        <v>6.4754000000000001E-3</v>
+      </c>
+      <c r="D105">
+        <v>6.4754000000000001E-3</v>
+      </c>
+      <c r="E105">
+        <v>6.4754000000000001E-3</v>
+      </c>
+      <c r="F105">
+        <v>6.4754000000000001E-3</v>
+      </c>
+      <c r="G105">
+        <v>6.4754000000000001E-3</v>
+      </c>
+      <c r="H105">
+        <v>6.4754000000000001E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>116</v>
+      </c>
+      <c r="C106">
+        <v>7.1618999999999997E-3</v>
+      </c>
+      <c r="D106">
+        <v>7.1618999999999997E-3</v>
+      </c>
+      <c r="E106">
+        <v>7.1618999999999997E-3</v>
+      </c>
+      <c r="F106">
+        <v>7.1618999999999997E-3</v>
+      </c>
+      <c r="G106">
+        <v>7.1618999999999997E-3</v>
+      </c>
+      <c r="H106">
+        <v>7.1618999999999997E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>117</v>
+      </c>
+      <c r="C107">
+        <v>7.7339000000000001E-3</v>
+      </c>
+      <c r="D107">
+        <v>7.7339000000000001E-3</v>
+      </c>
+      <c r="E107">
+        <v>7.7339000000000001E-3</v>
+      </c>
+      <c r="F107">
+        <v>7.7339000000000001E-3</v>
+      </c>
+      <c r="G107">
+        <v>7.7339000000000001E-3</v>
+      </c>
+      <c r="H107">
+        <v>7.7339000000000001E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>118</v>
+      </c>
+      <c r="C108">
+        <v>8.1618000000000003E-3</v>
+      </c>
+      <c r="D108">
+        <v>8.1618000000000003E-3</v>
+      </c>
+      <c r="E108">
+        <v>8.1618000000000003E-3</v>
+      </c>
+      <c r="F108">
+        <v>8.1618000000000003E-3</v>
+      </c>
+      <c r="G108">
+        <v>8.1618000000000003E-3</v>
+      </c>
+      <c r="H108">
+        <v>8.1618000000000003E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>119</v>
+      </c>
+      <c r="C109">
+        <v>8.4247000000000002E-3</v>
+      </c>
+      <c r="D109">
+        <v>8.4247000000000002E-3</v>
+      </c>
+      <c r="E109">
+        <v>8.4247000000000002E-3</v>
+      </c>
+      <c r="F109">
+        <v>8.4247000000000002E-3</v>
+      </c>
+      <c r="G109">
+        <v>8.4247000000000002E-3</v>
+      </c>
+      <c r="H109">
+        <v>8.4247000000000002E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110">
+        <v>8.5109999999999995E-3</v>
+      </c>
+      <c r="D110">
+        <v>8.5109999999999995E-3</v>
+      </c>
+      <c r="E110">
+        <v>8.5109999999999995E-3</v>
+      </c>
+      <c r="F110">
+        <v>8.5109999999999995E-3</v>
+      </c>
+      <c r="G110">
+        <v>8.5109999999999995E-3</v>
+      </c>
+      <c r="H110">
+        <v>8.5109999999999995E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111">
+        <v>8.4192999999999994E-3</v>
+      </c>
+      <c r="D111">
+        <v>8.4192999999999994E-3</v>
+      </c>
+      <c r="E111">
+        <v>8.4192999999999994E-3</v>
+      </c>
+      <c r="F111">
+        <v>8.4192999999999994E-3</v>
+      </c>
+      <c r="G111">
+        <v>8.4192999999999994E-3</v>
+      </c>
+      <c r="H111">
+        <v>8.4192999999999994E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112">
+        <v>8.1574000000000004E-3</v>
+      </c>
+      <c r="D112">
+        <v>8.1574000000000004E-3</v>
+      </c>
+      <c r="E112">
+        <v>8.1574000000000004E-3</v>
+      </c>
+      <c r="F112">
+        <v>8.1574000000000004E-3</v>
+      </c>
+      <c r="G112">
+        <v>8.1574000000000004E-3</v>
+      </c>
+      <c r="H112">
+        <v>8.1574000000000004E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113">
+        <v>7.7425000000000003E-3</v>
+      </c>
+      <c r="D113">
+        <v>7.7425000000000003E-3</v>
+      </c>
+      <c r="E113">
+        <v>7.7425000000000003E-3</v>
+      </c>
+      <c r="F113">
+        <v>7.7425000000000003E-3</v>
+      </c>
+      <c r="G113">
+        <v>7.7425000000000003E-3</v>
+      </c>
+      <c r="H113">
+        <v>7.7425000000000003E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114">
+        <v>7.1989999999999997E-3</v>
+      </c>
+      <c r="D114">
+        <v>7.1989999999999997E-3</v>
+      </c>
+      <c r="E114">
+        <v>7.1989999999999997E-3</v>
+      </c>
+      <c r="F114">
+        <v>7.1989999999999997E-3</v>
+      </c>
+      <c r="G114">
+        <v>7.1989999999999997E-3</v>
+      </c>
+      <c r="H114">
+        <v>7.1989999999999997E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>125</v>
+      </c>
+      <c r="C115">
+        <v>6.5573999999999997E-3</v>
+      </c>
+      <c r="D115">
+        <v>6.5573999999999997E-3</v>
+      </c>
+      <c r="E115">
+        <v>6.5573999999999997E-3</v>
+      </c>
+      <c r="F115">
+        <v>6.5573999999999997E-3</v>
+      </c>
+      <c r="G115">
+        <v>6.5573999999999997E-3</v>
+      </c>
+      <c r="H115">
+        <v>6.5573999999999997E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>126</v>
+      </c>
+      <c r="C116">
+        <v>5.8520000000000004E-3</v>
+      </c>
+      <c r="D116">
+        <v>5.8520000000000004E-3</v>
+      </c>
+      <c r="E116">
+        <v>5.8520000000000004E-3</v>
+      </c>
+      <c r="F116">
+        <v>5.8520000000000004E-3</v>
+      </c>
+      <c r="G116">
+        <v>5.8520000000000004E-3</v>
+      </c>
+      <c r="H116">
+        <v>5.8520000000000004E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>127</v>
+      </c>
+      <c r="C117">
+        <v>5.1187000000000003E-3</v>
+      </c>
+      <c r="D117">
+        <v>5.1187000000000003E-3</v>
+      </c>
+      <c r="E117">
+        <v>5.1187000000000003E-3</v>
+      </c>
+      <c r="F117">
+        <v>5.1187000000000003E-3</v>
+      </c>
+      <c r="G117">
+        <v>5.1187000000000003E-3</v>
+      </c>
+      <c r="H117">
+        <v>5.1187000000000003E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C118">
+        <v>4.3930999999999996E-3</v>
+      </c>
+      <c r="D118">
+        <v>4.3930999999999996E-3</v>
+      </c>
+      <c r="E118">
+        <v>4.3930999999999996E-3</v>
+      </c>
+      <c r="F118">
+        <v>4.3930999999999996E-3</v>
+      </c>
+      <c r="G118">
+        <v>4.3930999999999996E-3</v>
+      </c>
+      <c r="H118">
+        <v>4.3930999999999996E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>129</v>
+      </c>
+      <c r="C119">
+        <v>3.7081000000000002E-3</v>
+      </c>
+      <c r="D119">
+        <v>3.7081000000000002E-3</v>
+      </c>
+      <c r="E119">
+        <v>3.7081000000000002E-3</v>
+      </c>
+      <c r="F119">
+        <v>3.7081000000000002E-3</v>
+      </c>
+      <c r="G119">
+        <v>3.7081000000000002E-3</v>
+      </c>
+      <c r="H119">
+        <v>3.7081000000000002E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
+        <v>130</v>
+      </c>
+      <c r="C120">
+        <v>3.0918999999999999E-3</v>
+      </c>
+      <c r="D120">
+        <v>3.0918999999999999E-3</v>
+      </c>
+      <c r="E120">
+        <v>3.0918999999999999E-3</v>
+      </c>
+      <c r="F120">
+        <v>3.0918999999999999E-3</v>
+      </c>
+      <c r="G120">
+        <v>3.0918999999999999E-3</v>
+      </c>
+      <c r="H120">
+        <v>3.0918999999999999E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>131</v>
+      </c>
+      <c r="C121">
+        <v>2.5672E-3</v>
+      </c>
+      <c r="D121">
+        <v>2.5672E-3</v>
+      </c>
+      <c r="E121">
+        <v>2.5672E-3</v>
+      </c>
+      <c r="F121">
+        <v>2.5672E-3</v>
+      </c>
+      <c r="G121">
+        <v>2.5672E-3</v>
+      </c>
+      <c r="H121">
+        <v>2.5672E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>22</v>
+      </c>
+      <c r="C123" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
+        <v>33</v>
+      </c>
+      <c r="D124" t="s">
+        <v>34</v>
+      </c>
+      <c r="E124" t="s">
+        <v>35</v>
+      </c>
+      <c r="F124" t="s">
+        <v>36</v>
+      </c>
+      <c r="G124" t="s">
+        <v>37</v>
+      </c>
+      <c r="H124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C125" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" t="s">
+        <v>13</v>
+      </c>
+      <c r="E125" t="s">
+        <v>13</v>
+      </c>
+      <c r="F125" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125" t="s">
+        <v>13</v>
+      </c>
+      <c r="H125" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
+        <v>47</v>
+      </c>
+      <c r="C127" s="1">
+        <v>3.4023999999999998E-6</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1.9740999999999999E-6</v>
+      </c>
+      <c r="E127" s="1">
+        <v>1.1392E-6</v>
+      </c>
+      <c r="F127" s="1">
+        <v>6.5741000000000001E-7</v>
+      </c>
+      <c r="G127" s="1">
+        <v>3.6395999999999998E-7</v>
+      </c>
+      <c r="H127" s="1">
+        <v>1.9186E-7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>48</v>
+      </c>
+      <c r="C128" s="1">
+        <v>7.5801999999999999E-6</v>
+      </c>
+      <c r="D128" s="1">
+        <v>5.7072000000000002E-6</v>
+      </c>
+      <c r="E128" s="1">
+        <v>3.1481E-6</v>
+      </c>
+      <c r="F128" s="1">
+        <v>1.6374E-6</v>
+      </c>
+      <c r="G128" s="1">
+        <v>8.5183000000000002E-7</v>
+      </c>
+      <c r="H128" s="1">
+        <v>4.3426999999999998E-7</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
+        <v>49</v>
+      </c>
+      <c r="C129" s="1">
+        <v>1.1551E-5</v>
+      </c>
+      <c r="D129" s="1">
+        <v>1.0981999999999999E-5</v>
+      </c>
+      <c r="E129" s="1">
+        <v>7.9960999999999996E-6</v>
+      </c>
+      <c r="F129" s="1">
+        <v>4.2809E-6</v>
+      </c>
+      <c r="G129" s="1">
+        <v>2.1001E-6</v>
+      </c>
+      <c r="H129" s="1">
+        <v>1.0231E-6</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>50</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1.5488000000000001E-5</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1.5489E-5</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1.4262E-5</v>
+      </c>
+      <c r="F130" s="1">
+        <v>1.0152999999999999E-5</v>
+      </c>
+      <c r="G130" s="1">
+        <v>5.3163999999999996E-6</v>
+      </c>
+      <c r="H130" s="1">
+        <v>2.5050000000000002E-6</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B131" t="s">
+        <v>51</v>
+      </c>
+      <c r="C131" s="1">
+        <v>1.9398E-5</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1.9459000000000001E-5</v>
+      </c>
+      <c r="E131" s="1">
+        <v>1.9145000000000001E-5</v>
+      </c>
+      <c r="F131" s="1">
+        <v>1.7249E-5</v>
+      </c>
+      <c r="G131" s="1">
+        <v>1.2065999999999999E-5</v>
+      </c>
+      <c r="H131" s="1">
+        <v>6.2033000000000004E-6</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
+        <v>52</v>
+      </c>
+      <c r="C132" s="1">
+        <v>2.3011E-5</v>
+      </c>
+      <c r="D132" s="1">
+        <v>2.3047000000000001E-5</v>
+      </c>
+      <c r="E132" s="1">
+        <v>2.2963E-5</v>
+      </c>
+      <c r="F132" s="1">
+        <v>2.2323999999999998E-5</v>
+      </c>
+      <c r="G132" s="1">
+        <v>1.9786E-5</v>
+      </c>
+      <c r="H132" s="1">
+        <v>1.3638999999999999E-5</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
+        <v>53</v>
+      </c>
+      <c r="C133" s="1">
+        <v>2.6058999999999999E-5</v>
+      </c>
+      <c r="D133" s="1">
+        <v>2.6075E-5</v>
+      </c>
+      <c r="E133" s="1">
+        <v>2.6044999999999999E-5</v>
+      </c>
+      <c r="F133" s="1">
+        <v>2.5812E-5</v>
+      </c>
+      <c r="G133" s="1">
+        <v>2.4856999999999999E-5</v>
+      </c>
+      <c r="H133" s="1">
+        <v>2.1736999999999999E-5</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>54</v>
+      </c>
+      <c r="C134" s="1">
+        <v>2.8337E-5</v>
+      </c>
+      <c r="D134" s="1">
+        <v>2.8342000000000001E-5</v>
+      </c>
+      <c r="E134" s="1">
+        <v>2.8326999999999998E-5</v>
+      </c>
+      <c r="F134" s="1">
+        <v>2.8229E-5</v>
+      </c>
+      <c r="G134" s="1">
+        <v>2.7849999999999999E-5</v>
+      </c>
+      <c r="H134" s="1">
+        <v>2.6602999999999999E-5</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B135" t="s">
+        <v>55</v>
+      </c>
+      <c r="C135" s="1">
+        <v>2.9692E-5</v>
+      </c>
+      <c r="D135" s="1">
+        <v>2.9694000000000001E-5</v>
+      </c>
+      <c r="E135" s="1">
+        <v>2.9686E-5</v>
+      </c>
+      <c r="F135" s="1">
+        <v>2.9640000000000001E-5</v>
+      </c>
+      <c r="G135" s="1">
+        <v>2.9475000000000002E-5</v>
+      </c>
+      <c r="H135" s="1">
+        <v>2.8958E-5</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>56</v>
+      </c>
+      <c r="C136" s="1">
+        <v>3.0031000000000001E-5</v>
+      </c>
+      <c r="D136" s="1">
+        <v>3.0031000000000001E-5</v>
+      </c>
+      <c r="E136" s="1">
+        <v>3.0026999999999999E-5</v>
+      </c>
+      <c r="F136" s="1">
+        <v>3.0005000000000002E-5</v>
+      </c>
+      <c r="G136" s="1">
+        <v>2.9929000000000001E-5</v>
+      </c>
+      <c r="H136" s="1">
+        <v>2.97E-5</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
+        <v>57</v>
+      </c>
+      <c r="C137" s="1">
+        <v>2.9311000000000001E-5</v>
+      </c>
+      <c r="D137" s="1">
+        <v>2.9311000000000001E-5</v>
+      </c>
+      <c r="E137" s="1">
+        <v>2.9308000000000001E-5</v>
+      </c>
+      <c r="F137" s="1">
+        <v>2.9297000000000001E-5</v>
+      </c>
+      <c r="G137" s="1">
+        <v>2.9261E-5</v>
+      </c>
+      <c r="H137" s="1">
+        <v>2.9156999999999999E-5</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
+        <v>87</v>
+      </c>
+      <c r="C138" s="1">
+        <v>2.7540000000000001E-5</v>
+      </c>
+      <c r="D138" s="1">
+        <v>2.7538999999999998E-5</v>
+      </c>
+      <c r="E138" s="1">
+        <v>2.7538E-5</v>
+      </c>
+      <c r="F138" s="1">
+        <v>2.7532999999999999E-5</v>
+      </c>
+      <c r="G138" s="1">
+        <v>2.7515999999999999E-5</v>
+      </c>
+      <c r="H138" s="1">
+        <v>2.7467E-5</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B139" t="s">
+        <v>88</v>
+      </c>
+      <c r="C139" s="1">
+        <v>2.4776000000000001E-5</v>
+      </c>
+      <c r="D139" s="1">
+        <v>2.4774999999999999E-5</v>
+      </c>
+      <c r="E139" s="1">
+        <v>2.4774999999999999E-5</v>
+      </c>
+      <c r="F139" s="1">
+        <v>2.4771999999999999E-5</v>
+      </c>
+      <c r="G139" s="1">
+        <v>2.4763999999999999E-5</v>
+      </c>
+      <c r="H139" s="1">
+        <v>2.4740999999999999E-5</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
+        <v>89</v>
+      </c>
+      <c r="C140" s="1">
+        <v>2.1121E-5</v>
+      </c>
+      <c r="D140" s="1">
+        <v>2.1121E-5</v>
+      </c>
+      <c r="E140" s="1">
+        <v>2.1121E-5</v>
+      </c>
+      <c r="F140" s="1">
+        <v>2.1120000000000001E-5</v>
+      </c>
+      <c r="G140" s="1">
+        <v>2.1115999999999999E-5</v>
+      </c>
+      <c r="H140" s="1">
+        <v>2.1104999999999999E-5</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B141" t="s">
+        <v>90</v>
+      </c>
+      <c r="C141" s="1">
+        <v>1.6718000000000002E-5</v>
+      </c>
+      <c r="D141" s="1">
+        <v>1.6718000000000002E-5</v>
+      </c>
+      <c r="E141" s="1">
+        <v>1.6718000000000002E-5</v>
+      </c>
+      <c r="F141" s="1">
+        <v>1.6718000000000002E-5</v>
+      </c>
+      <c r="G141" s="1">
+        <v>1.6716000000000001E-5</v>
+      </c>
+      <c r="H141" s="1">
+        <v>1.6711E-5</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B142" t="s">
+        <v>91</v>
+      </c>
+      <c r="C142" s="1">
+        <v>1.1739999999999999E-5</v>
+      </c>
+      <c r="D142" s="1">
+        <v>1.1739999999999999E-5</v>
+      </c>
+      <c r="E142" s="1">
+        <v>1.1739999999999999E-5</v>
+      </c>
+      <c r="F142" s="1">
+        <v>1.1739999999999999E-5</v>
+      </c>
+      <c r="G142" s="1">
+        <v>1.1739000000000001E-5</v>
+      </c>
+      <c r="H142" s="1">
+        <v>1.1737E-5</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B143" t="s">
+        <v>92</v>
+      </c>
+      <c r="C143" s="1">
+        <v>6.3821999999999996E-6</v>
+      </c>
+      <c r="D143" s="1">
+        <v>6.3821999999999996E-6</v>
+      </c>
+      <c r="E143" s="1">
+        <v>6.3821000000000003E-6</v>
+      </c>
+      <c r="F143" s="1">
+        <v>6.3820000000000001E-6</v>
+      </c>
+      <c r="G143" s="1">
+        <v>6.3816E-6</v>
+      </c>
+      <c r="H143" s="1">
+        <v>6.3806000000000004E-6</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B144" t="s">
+        <v>93</v>
+      </c>
+      <c r="C144" s="1">
+        <v>8.5252000000000001E-7</v>
+      </c>
+      <c r="D144" s="1">
+        <v>8.5252000000000001E-7</v>
+      </c>
+      <c r="E144" s="1">
+        <v>8.5249999999999999E-7</v>
+      </c>
+      <c r="F144" s="1">
+        <v>8.5244999999999999E-7</v>
+      </c>
+      <c r="G144" s="1">
+        <v>8.5229000000000002E-7</v>
+      </c>
+      <c r="H144" s="1">
+        <v>8.5183999999999998E-7</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
+        <v>94</v>
+      </c>
+      <c r="C145" s="1">
+        <v>-4.6381999999999999E-6</v>
+      </c>
+      <c r="D145" s="1">
+        <v>-4.6381999999999999E-6</v>
+      </c>
+      <c r="E145" s="1">
+        <v>-4.6381999999999999E-6</v>
+      </c>
+      <c r="F145" s="1">
+        <v>-4.6381999999999999E-6</v>
+      </c>
+      <c r="G145" s="1">
+        <v>-4.6383000000000001E-6</v>
+      </c>
+      <c r="H145" s="1">
+        <v>-4.6384999999999997E-6</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B146" t="s">
+        <v>95</v>
+      </c>
+      <c r="C146" s="1">
+        <v>-9.8871000000000006E-6</v>
+      </c>
+      <c r="D146" s="1">
+        <v>-9.8871000000000006E-6</v>
+      </c>
+      <c r="E146" s="1">
+        <v>-9.8871000000000006E-6</v>
+      </c>
+      <c r="F146" s="1">
+        <v>-9.8871000000000006E-6</v>
+      </c>
+      <c r="G146" s="1">
+        <v>-9.8871000000000006E-6</v>
+      </c>
+      <c r="H146" s="1">
+        <v>-9.8872000000000008E-6</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B147" t="s">
+        <v>96</v>
+      </c>
+      <c r="C147" s="1">
+        <v>-1.4708999999999999E-5</v>
+      </c>
+      <c r="D147" s="1">
+        <v>-1.4708999999999999E-5</v>
+      </c>
+      <c r="E147" s="1">
+        <v>-1.4708999999999999E-5</v>
+      </c>
+      <c r="F147" s="1">
+        <v>-1.4708999999999999E-5</v>
+      </c>
+      <c r="G147" s="1">
+        <v>-1.4708999999999999E-5</v>
+      </c>
+      <c r="H147" s="1">
+        <v>-1.4708999999999999E-5</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
+        <v>97</v>
+      </c>
+      <c r="C148" s="1">
+        <v>-1.8943000000000001E-5</v>
+      </c>
+      <c r="D148" s="1">
+        <v>-1.8943000000000001E-5</v>
+      </c>
+      <c r="E148" s="1">
+        <v>-1.8943000000000001E-5</v>
+      </c>
+      <c r="F148" s="1">
+        <v>-1.8943000000000001E-5</v>
+      </c>
+      <c r="G148" s="1">
+        <v>-1.8943000000000001E-5</v>
+      </c>
+      <c r="H148" s="1">
+        <v>-1.8943000000000001E-5</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B149" t="s">
+        <v>98</v>
+      </c>
+      <c r="C149" s="1">
+        <v>-2.2463000000000002E-5</v>
+      </c>
+      <c r="D149" s="1">
+        <v>-2.2463000000000002E-5</v>
+      </c>
+      <c r="E149" s="1">
+        <v>-2.2463000000000002E-5</v>
+      </c>
+      <c r="F149" s="1">
+        <v>-2.2463000000000002E-5</v>
+      </c>
+      <c r="G149" s="1">
+        <v>-2.2463000000000002E-5</v>
+      </c>
+      <c r="H149" s="1">
+        <v>-2.2463000000000002E-5</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B150" t="s">
+        <v>99</v>
+      </c>
+      <c r="C150" s="1">
+        <v>-2.5177999999999998E-5</v>
+      </c>
+      <c r="D150" s="1">
+        <v>-2.5177999999999998E-5</v>
+      </c>
+      <c r="E150" s="1">
+        <v>-2.5177999999999998E-5</v>
+      </c>
+      <c r="F150" s="1">
+        <v>-2.5177999999999998E-5</v>
+      </c>
+      <c r="G150" s="1">
+        <v>-2.5177999999999998E-5</v>
+      </c>
+      <c r="H150" s="1">
+        <v>-2.5177999999999998E-5</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
+        <v>100</v>
+      </c>
+      <c r="C151" s="1">
+        <v>-2.7039E-5</v>
+      </c>
+      <c r="D151" s="1">
+        <v>-2.7039E-5</v>
+      </c>
+      <c r="E151" s="1">
+        <v>-2.7039E-5</v>
+      </c>
+      <c r="F151" s="1">
+        <v>-2.7039E-5</v>
+      </c>
+      <c r="G151" s="1">
+        <v>-2.7039E-5</v>
+      </c>
+      <c r="H151" s="1">
+        <v>-2.7039E-5</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>101</v>
+      </c>
+      <c r="C152" s="1">
+        <v>-2.8036000000000001E-5</v>
+      </c>
+      <c r="D152" s="1">
+        <v>-2.8036000000000001E-5</v>
+      </c>
+      <c r="E152" s="1">
+        <v>-2.8036000000000001E-5</v>
+      </c>
+      <c r="F152" s="1">
+        <v>-2.8036000000000001E-5</v>
+      </c>
+      <c r="G152" s="1">
+        <v>-2.8036000000000001E-5</v>
+      </c>
+      <c r="H152" s="1">
+        <v>-2.8036000000000001E-5</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B153" t="s">
+        <v>102</v>
+      </c>
+      <c r="C153" s="1">
+        <v>-2.8201E-5</v>
+      </c>
+      <c r="D153" s="1">
+        <v>-2.8201E-5</v>
+      </c>
+      <c r="E153" s="1">
+        <v>-2.8201E-5</v>
+      </c>
+      <c r="F153" s="1">
+        <v>-2.8201E-5</v>
+      </c>
+      <c r="G153" s="1">
+        <v>-2.8201E-5</v>
+      </c>
+      <c r="H153" s="1">
+        <v>-2.8201E-5</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B154" t="s">
+        <v>103</v>
+      </c>
+      <c r="C154" s="1">
+        <v>-2.7600999999999999E-5</v>
+      </c>
+      <c r="D154" s="1">
+        <v>-2.7600999999999999E-5</v>
+      </c>
+      <c r="E154" s="1">
+        <v>-2.7600999999999999E-5</v>
+      </c>
+      <c r="F154" s="1">
+        <v>-2.7600999999999999E-5</v>
+      </c>
+      <c r="G154" s="1">
+        <v>-2.7600999999999999E-5</v>
+      </c>
+      <c r="H154" s="1">
+        <v>-2.7600999999999999E-5</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
+        <v>104</v>
+      </c>
+      <c r="C155" s="1">
+        <v>-2.6333999999999999E-5</v>
+      </c>
+      <c r="D155" s="1">
+        <v>-2.6333999999999999E-5</v>
+      </c>
+      <c r="E155" s="1">
+        <v>-2.6333999999999999E-5</v>
+      </c>
+      <c r="F155" s="1">
+        <v>-2.6333999999999999E-5</v>
+      </c>
+      <c r="G155" s="1">
+        <v>-2.6333999999999999E-5</v>
+      </c>
+      <c r="H155" s="1">
+        <v>-2.6333999999999999E-5</v>
+      </c>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B156" t="s">
+        <v>105</v>
+      </c>
+      <c r="C156" s="1">
+        <v>-2.4522E-5</v>
+      </c>
+      <c r="D156" s="1">
+        <v>-2.4522E-5</v>
+      </c>
+      <c r="E156" s="1">
+        <v>-2.4522E-5</v>
+      </c>
+      <c r="F156" s="1">
+        <v>-2.4522E-5</v>
+      </c>
+      <c r="G156" s="1">
+        <v>-2.4522E-5</v>
+      </c>
+      <c r="H156" s="1">
+        <v>-2.4522E-5</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B157" t="s">
+        <v>106</v>
+      </c>
+      <c r="C157" s="1">
+        <v>-2.2306999999999998E-5</v>
+      </c>
+      <c r="D157" s="1">
+        <v>-2.2306999999999998E-5</v>
+      </c>
+      <c r="E157" s="1">
+        <v>-2.2306999999999998E-5</v>
+      </c>
+      <c r="F157" s="1">
+        <v>-2.2306999999999998E-5</v>
+      </c>
+      <c r="G157" s="1">
+        <v>-2.2306999999999998E-5</v>
+      </c>
+      <c r="H157" s="1">
+        <v>-2.2306999999999998E-5</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
+        <v>107</v>
+      </c>
+      <c r="C158" s="1">
+        <v>-1.9834999999999999E-5</v>
+      </c>
+      <c r="D158" s="1">
+        <v>-1.9834999999999999E-5</v>
+      </c>
+      <c r="E158" s="1">
+        <v>-1.9834999999999999E-5</v>
+      </c>
+      <c r="F158" s="1">
+        <v>-1.9834999999999999E-5</v>
+      </c>
+      <c r="G158" s="1">
+        <v>-1.9834999999999999E-5</v>
+      </c>
+      <c r="H158" s="1">
+        <v>-1.9834999999999999E-5</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>108</v>
+      </c>
+      <c r="C159" s="1">
+        <v>-1.7255999999999999E-5</v>
+      </c>
+      <c r="D159" s="1">
+        <v>-1.7255999999999999E-5</v>
+      </c>
+      <c r="E159" s="1">
+        <v>-1.7255999999999999E-5</v>
+      </c>
+      <c r="F159" s="1">
+        <v>-1.7255999999999999E-5</v>
+      </c>
+      <c r="G159" s="1">
+        <v>-1.7255999999999999E-5</v>
+      </c>
+      <c r="H159" s="1">
+        <v>-1.7255999999999999E-5</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B160" t="s">
+        <v>109</v>
+      </c>
+      <c r="C160" s="1">
+        <v>-1.4712000000000001E-5</v>
+      </c>
+      <c r="D160" s="1">
+        <v>-1.4712000000000001E-5</v>
+      </c>
+      <c r="E160" s="1">
+        <v>-1.4712000000000001E-5</v>
+      </c>
+      <c r="F160" s="1">
+        <v>-1.4712000000000001E-5</v>
+      </c>
+      <c r="G160" s="1">
+        <v>-1.4712000000000001E-5</v>
+      </c>
+      <c r="H160" s="1">
+        <v>-1.4712000000000001E-5</v>
+      </c>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
+        <v>110</v>
+      </c>
+      <c r="C161" s="1">
+        <v>-1.2330000000000001E-5</v>
+      </c>
+      <c r="D161" s="1">
+        <v>-1.2330000000000001E-5</v>
+      </c>
+      <c r="E161" s="1">
+        <v>-1.2330000000000001E-5</v>
+      </c>
+      <c r="F161" s="1">
+        <v>-1.2330000000000001E-5</v>
+      </c>
+      <c r="G161" s="1">
+        <v>-1.2330000000000001E-5</v>
+      </c>
+      <c r="H161" s="1">
+        <v>-1.2330000000000001E-5</v>
+      </c>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>111</v>
+      </c>
+      <c r="C162" s="1">
+        <v>-1.0215E-5</v>
+      </c>
+      <c r="D162" s="1">
+        <v>-1.0215E-5</v>
+      </c>
+      <c r="E162" s="1">
+        <v>-1.0215E-5</v>
+      </c>
+      <c r="F162" s="1">
+        <v>-1.0215E-5</v>
+      </c>
+      <c r="G162" s="1">
+        <v>-1.0215E-5</v>
+      </c>
+      <c r="H162" s="1">
+        <v>-1.0215E-5</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>112</v>
+      </c>
+      <c r="C163" s="1">
+        <v>-8.4478000000000007E-6</v>
+      </c>
+      <c r="D163" s="1">
+        <v>-8.4478000000000007E-6</v>
+      </c>
+      <c r="E163" s="1">
+        <v>-8.4478000000000007E-6</v>
+      </c>
+      <c r="F163" s="1">
+        <v>-8.4478000000000007E-6</v>
+      </c>
+      <c r="G163" s="1">
+        <v>-8.4478000000000007E-6</v>
+      </c>
+      <c r="H163" s="1">
+        <v>-8.4478000000000007E-6</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>113</v>
+      </c>
+      <c r="C164" s="1">
+        <v>-7.0806999999999998E-6</v>
+      </c>
+      <c r="D164" s="1">
+        <v>-7.0806999999999998E-6</v>
+      </c>
+      <c r="E164" s="1">
+        <v>-7.0806999999999998E-6</v>
+      </c>
+      <c r="F164" s="1">
+        <v>-7.0806999999999998E-6</v>
+      </c>
+      <c r="G164" s="1">
+        <v>-7.0806999999999998E-6</v>
+      </c>
+      <c r="H164" s="1">
+        <v>-7.0806999999999998E-6</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
+        <v>114</v>
+      </c>
+      <c r="C165" s="1">
+        <v>-6.1357000000000004E-6</v>
+      </c>
+      <c r="D165" s="1">
+        <v>-6.1357000000000004E-6</v>
+      </c>
+      <c r="E165" s="1">
+        <v>-6.1357000000000004E-6</v>
+      </c>
+      <c r="F165" s="1">
+        <v>-6.1357000000000004E-6</v>
+      </c>
+      <c r="G165" s="1">
+        <v>-6.1357000000000004E-6</v>
+      </c>
+      <c r="H165" s="1">
+        <v>-6.1357000000000004E-6</v>
+      </c>
+    </row>
+    <row r="166" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B166" t="s">
+        <v>115</v>
+      </c>
+      <c r="C166" s="1">
+        <v>-5.6059E-6</v>
+      </c>
+      <c r="D166" s="1">
+        <v>-5.6059E-6</v>
+      </c>
+      <c r="E166" s="1">
+        <v>-5.6059E-6</v>
+      </c>
+      <c r="F166" s="1">
+        <v>-5.6059E-6</v>
+      </c>
+      <c r="G166" s="1">
+        <v>-5.6059E-6</v>
+      </c>
+      <c r="H166" s="1">
+        <v>-5.6059E-6</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B167" t="s">
+        <v>116</v>
+      </c>
+      <c r="C167" s="1">
+        <v>-5.4568E-6</v>
+      </c>
+      <c r="D167" s="1">
+        <v>-5.4568E-6</v>
+      </c>
+      <c r="E167" s="1">
+        <v>-5.4568E-6</v>
+      </c>
+      <c r="F167" s="1">
+        <v>-5.4568E-6</v>
+      </c>
+      <c r="G167" s="1">
+        <v>-5.4568E-6</v>
+      </c>
+      <c r="H167" s="1">
+        <v>-5.4568E-6</v>
+      </c>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B168" t="s">
+        <v>117</v>
+      </c>
+      <c r="C168" s="1">
+        <v>-5.6307000000000001E-6</v>
+      </c>
+      <c r="D168" s="1">
+        <v>-5.6307000000000001E-6</v>
+      </c>
+      <c r="E168" s="1">
+        <v>-5.6307000000000001E-6</v>
+      </c>
+      <c r="F168" s="1">
+        <v>-5.6307000000000001E-6</v>
+      </c>
+      <c r="G168" s="1">
+        <v>-5.6307000000000001E-6</v>
+      </c>
+      <c r="H168" s="1">
+        <v>-5.6307000000000001E-6</v>
+      </c>
+    </row>
+    <row r="169" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B169" t="s">
+        <v>118</v>
+      </c>
+      <c r="C169" s="1">
+        <v>-6.0509E-6</v>
+      </c>
+      <c r="D169" s="1">
+        <v>-6.0509E-6</v>
+      </c>
+      <c r="E169" s="1">
+        <v>-6.0509E-6</v>
+      </c>
+      <c r="F169" s="1">
+        <v>-6.0509E-6</v>
+      </c>
+      <c r="G169" s="1">
+        <v>-6.0509E-6</v>
+      </c>
+      <c r="H169" s="1">
+        <v>-6.0509E-6</v>
+      </c>
+    </row>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
+        <v>119</v>
+      </c>
+      <c r="C170" s="1">
+        <v>-6.6274999999999996E-6</v>
+      </c>
+      <c r="D170" s="1">
+        <v>-6.6274999999999996E-6</v>
+      </c>
+      <c r="E170" s="1">
+        <v>-6.6274999999999996E-6</v>
+      </c>
+      <c r="F170" s="1">
+        <v>-6.6274999999999996E-6</v>
+      </c>
+      <c r="G170" s="1">
+        <v>-6.6274999999999996E-6</v>
+      </c>
+      <c r="H170" s="1">
+        <v>-6.6274999999999996E-6</v>
+      </c>
+    </row>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B171" t="s">
+        <v>120</v>
+      </c>
+      <c r="C171" s="1">
+        <v>-7.2640999999999996E-6</v>
+      </c>
+      <c r="D171" s="1">
+        <v>-7.2640999999999996E-6</v>
+      </c>
+      <c r="E171" s="1">
+        <v>-7.2640999999999996E-6</v>
+      </c>
+      <c r="F171" s="1">
+        <v>-7.2640999999999996E-6</v>
+      </c>
+      <c r="G171" s="1">
+        <v>-7.2640999999999996E-6</v>
+      </c>
+      <c r="H171" s="1">
+        <v>-7.2640999999999996E-6</v>
+      </c>
+    </row>
+    <row r="172" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B172" t="s">
+        <v>121</v>
+      </c>
+      <c r="C172" s="1">
+        <v>-7.8635000000000002E-6</v>
+      </c>
+      <c r="D172" s="1">
+        <v>-7.8635000000000002E-6</v>
+      </c>
+      <c r="E172" s="1">
+        <v>-7.8635000000000002E-6</v>
+      </c>
+      <c r="F172" s="1">
+        <v>-7.8635000000000002E-6</v>
+      </c>
+      <c r="G172" s="1">
+        <v>-7.8635000000000002E-6</v>
+      </c>
+      <c r="H172" s="1">
+        <v>-7.8635000000000002E-6</v>
+      </c>
+    </row>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B173" t="s">
+        <v>122</v>
+      </c>
+      <c r="C173" s="1">
+        <v>-8.3347E-6</v>
+      </c>
+      <c r="D173" s="1">
+        <v>-8.3347E-6</v>
+      </c>
+      <c r="E173" s="1">
+        <v>-8.3347E-6</v>
+      </c>
+      <c r="F173" s="1">
+        <v>-8.3347E-6</v>
+      </c>
+      <c r="G173" s="1">
+        <v>-8.3347E-6</v>
+      </c>
+      <c r="H173" s="1">
+        <v>-8.3347E-6</v>
+      </c>
+    </row>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B174" t="s">
+        <v>123</v>
+      </c>
+      <c r="C174" s="1">
+        <v>-8.5975000000000003E-6</v>
+      </c>
+      <c r="D174" s="1">
+        <v>-8.5975000000000003E-6</v>
+      </c>
+      <c r="E174" s="1">
+        <v>-8.5975000000000003E-6</v>
+      </c>
+      <c r="F174" s="1">
+        <v>-8.5975000000000003E-6</v>
+      </c>
+      <c r="G174" s="1">
+        <v>-8.5975000000000003E-6</v>
+      </c>
+      <c r="H174" s="1">
+        <v>-8.5975000000000003E-6</v>
+      </c>
+    </row>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B175" t="s">
+        <v>124</v>
+      </c>
+      <c r="C175" s="1">
+        <v>-8.5881E-6</v>
+      </c>
+      <c r="D175" s="1">
+        <v>-8.5881E-6</v>
+      </c>
+      <c r="E175" s="1">
+        <v>-8.5881E-6</v>
+      </c>
+      <c r="F175" s="1">
+        <v>-8.5881E-6</v>
+      </c>
+      <c r="G175" s="1">
+        <v>-8.5881E-6</v>
+      </c>
+      <c r="H175" s="1">
+        <v>-8.5881E-6</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B176" t="s">
+        <v>125</v>
+      </c>
+      <c r="C176" s="1">
+        <v>-8.2621000000000001E-6</v>
+      </c>
+      <c r="D176" s="1">
+        <v>-8.2621000000000001E-6</v>
+      </c>
+      <c r="E176" s="1">
+        <v>-8.2621000000000001E-6</v>
+      </c>
+      <c r="F176" s="1">
+        <v>-8.2621000000000001E-6</v>
+      </c>
+      <c r="G176" s="1">
+        <v>-8.2621000000000001E-6</v>
+      </c>
+      <c r="H176" s="1">
+        <v>-8.2621000000000001E-6</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B177" t="s">
+        <v>126</v>
+      </c>
+      <c r="C177" s="1">
+        <v>-7.5970000000000003E-6</v>
+      </c>
+      <c r="D177" s="1">
+        <v>-7.5970000000000003E-6</v>
+      </c>
+      <c r="E177" s="1">
+        <v>-7.5970000000000003E-6</v>
+      </c>
+      <c r="F177" s="1">
+        <v>-7.5970000000000003E-6</v>
+      </c>
+      <c r="G177" s="1">
+        <v>-7.5970000000000003E-6</v>
+      </c>
+      <c r="H177" s="1">
+        <v>-7.5970000000000003E-6</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B178" t="s">
+        <v>127</v>
+      </c>
+      <c r="C178" s="1">
+        <v>-6.5929E-6</v>
+      </c>
+      <c r="D178" s="1">
+        <v>-6.5929E-6</v>
+      </c>
+      <c r="E178" s="1">
+        <v>-6.5929E-6</v>
+      </c>
+      <c r="F178" s="1">
+        <v>-6.5929E-6</v>
+      </c>
+      <c r="G178" s="1">
+        <v>-6.5929E-6</v>
+      </c>
+      <c r="H178" s="1">
+        <v>-6.5929E-6</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B179" t="s">
+        <v>128</v>
+      </c>
+      <c r="C179" s="1">
+        <v>-5.2719000000000003E-6</v>
+      </c>
+      <c r="D179" s="1">
+        <v>-5.2719000000000003E-6</v>
+      </c>
+      <c r="E179" s="1">
+        <v>-5.2719000000000003E-6</v>
+      </c>
+      <c r="F179" s="1">
+        <v>-5.2719000000000003E-6</v>
+      </c>
+      <c r="G179" s="1">
+        <v>-5.2719000000000003E-6</v>
+      </c>
+      <c r="H179" s="1">
+        <v>-5.2719000000000003E-6</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B180" t="s">
+        <v>129</v>
+      </c>
+      <c r="C180" s="1">
+        <v>-3.6764999999999999E-6</v>
+      </c>
+      <c r="D180" s="1">
+        <v>-3.6764999999999999E-6</v>
+      </c>
+      <c r="E180" s="1">
+        <v>-3.6764999999999999E-6</v>
+      </c>
+      <c r="F180" s="1">
+        <v>-3.6764999999999999E-6</v>
+      </c>
+      <c r="G180" s="1">
+        <v>-3.6764999999999999E-6</v>
+      </c>
+      <c r="H180" s="1">
+        <v>-3.6764999999999999E-6</v>
+      </c>
+    </row>
+    <row r="181" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B181" t="s">
+        <v>130</v>
+      </c>
+      <c r="C181" s="1">
+        <v>-1.8664E-6</v>
+      </c>
+      <c r="D181" s="1">
+        <v>-1.8664E-6</v>
+      </c>
+      <c r="E181" s="1">
+        <v>-1.8664E-6</v>
+      </c>
+      <c r="F181" s="1">
+        <v>-1.8664E-6</v>
+      </c>
+      <c r="G181" s="1">
+        <v>-1.8664E-6</v>
+      </c>
+      <c r="H181" s="1">
+        <v>-1.8664E-6</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B182" t="s">
+        <v>131</v>
+      </c>
+      <c r="C182" s="1">
+        <v>8.5684000000000001E-8</v>
+      </c>
+      <c r="D182" s="1">
+        <v>8.5684000000000001E-8</v>
+      </c>
+      <c r="E182" s="1">
+        <v>8.5684000000000001E-8</v>
+      </c>
+      <c r="F182" s="1">
+        <v>8.5684000000000001E-8</v>
+      </c>
+      <c r="G182" s="1">
+        <v>8.5684000000000001E-8</v>
+      </c>
+      <c r="H182" s="1">
+        <v>8.5684000000000001E-8</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B186" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="187" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B187" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B189" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="190" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B190" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="191" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B191" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="192" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B192" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B193" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B194" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B195" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B196" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B197" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>